<commit_message>
cap Statements, search parameters all in FSH
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-NatlDirEndpointQry-HealthcareService.xlsx
+++ b/output/StructureDefinition-NatlDirEndpointQry-HealthcareService.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AK$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AK$79</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2624" uniqueCount="466">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-02-03T10:48:00-05:00</t>
+    <t>2022-03-09T14:32:46-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -593,6 +593,20 @@
   </si>
   <si>
     <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/rating}
+</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
   </si>
   <si>
     <t>newpatients</t>
@@ -608,10 +622,6 @@
     <t>New Patients indicates whether new patients are being accepted in general, or from a specific network.   
               This extension is included in the PractitionerRole, HealthcareService, and Location profiles.  
               This provides needed flexibility for specifying whether a provider accepts new patients by location and network.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1
-</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
@@ -1771,7 +1781,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK78"/>
+  <dimension ref="A1:AK79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3635,7 +3645,7 @@
         <v>188</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3695,10 +3705,10 @@
         <v>76</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>191</v>
+        <v>110</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>74</v>
@@ -3712,14 +3722,14 @@
         <v>182</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>74</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>76</v>
@@ -3734,13 +3744,13 @@
         <v>74</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="K19" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>195</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3800,10 +3810,10 @@
         <v>76</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>74</v>
@@ -3812,32 +3822,34 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>195</v>
+      </c>
       <c r="C20" t="s" s="2">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>74</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>102</v>
+        <v>196</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>197</v>
@@ -3845,12 +3857,8 @@
       <c r="L20" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="M20" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>199</v>
-      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>74</v>
       </c>
@@ -3898,7 +3906,7 @@
         <v>74</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>75</v>
@@ -3907,13 +3915,13 @@
         <v>76</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>74</v>
+        <v>189</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>110</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>181</v>
+        <v>74</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>74</v>
@@ -3921,11 +3929,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3938,22 +3946,26 @@
         <v>74</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N21" t="s" s="2">
         <v>202</v>
       </c>
-      <c r="K21" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>74</v>
       </c>
@@ -4001,7 +4013,7 @@
         <v>74</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>75</v>
@@ -4013,18 +4025,18 @@
         <v>74</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>206</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4035,7 +4047,7 @@
         <v>75</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>74</v>
@@ -4044,16 +4056,16 @@
         <v>74</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -4104,41 +4116,41 @@
         <v>74</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>99</v>
+        <v>208</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>74</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>74</v>
@@ -4150,17 +4162,15 @@
         <v>74</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>74</v>
@@ -4197,31 +4207,31 @@
         <v>74</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="AC23" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>99</v>
@@ -4232,43 +4242,41 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>74</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>210</v>
+        <v>103</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>211</v>
+        <v>104</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>213</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>74</v>
       </c>
@@ -4292,54 +4300,54 @@
         <v>74</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>214</v>
+        <v>74</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>215</v>
+        <v>74</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>216</v>
+        <v>74</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="AC24" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>217</v>
+        <v>109</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>218</v>
+        <v>99</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4353,28 +4361,28 @@
         <v>82</v>
       </c>
       <c r="G25" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="H25" t="s" s="2">
-        <v>74</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>83</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>74</v>
@@ -4399,13 +4407,13 @@
         <v>74</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>74</v>
@@ -4423,7 +4431,7 @@
         <v>74</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>75</v>
@@ -4438,15 +4446,15 @@
         <v>94</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4460,7 +4468,7 @@
         <v>82</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>74</v>
@@ -4469,19 +4477,19 @@
         <v>83</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>74</v>
@@ -4494,7 +4502,7 @@
         <v>74</v>
       </c>
       <c r="S26" t="s" s="2">
-        <v>233</v>
+        <v>74</v>
       </c>
       <c r="T26" t="s" s="2">
         <v>74</v>
@@ -4506,13 +4514,13 @@
         <v>74</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>74</v>
+        <v>228</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>74</v>
+        <v>229</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>74</v>
@@ -4530,7 +4538,7 @@
         <v>74</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>75</v>
@@ -4545,15 +4553,15 @@
         <v>94</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4567,7 +4575,7 @@
         <v>82</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>74</v>
@@ -4576,18 +4584,20 @@
         <v>83</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="N27" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>235</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>74</v>
       </c>
@@ -4599,7 +4609,7 @@
         <v>74</v>
       </c>
       <c r="S27" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="T27" t="s" s="2">
         <v>74</v>
@@ -4635,7 +4645,7 @@
         <v>74</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>75</v>
@@ -4650,15 +4660,15 @@
         <v>94</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4672,7 +4682,7 @@
         <v>82</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>74</v>
@@ -4681,15 +4691,17 @@
         <v>83</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>244</v>
+        <v>84</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="M28" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>242</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>74</v>
@@ -4702,7 +4714,7 @@
         <v>74</v>
       </c>
       <c r="S28" t="s" s="2">
-        <v>74</v>
+        <v>243</v>
       </c>
       <c r="T28" t="s" s="2">
         <v>74</v>
@@ -4738,7 +4750,7 @@
         <v>74</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>75</v>
@@ -4753,7 +4765,7 @@
         <v>94</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>74</v>
@@ -4761,7 +4773,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4784,17 +4796,15 @@
         <v>83</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>253</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>74</v>
@@ -4843,7 +4853,7 @@
         <v>74</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>75</v>
@@ -4858,15 +4868,15 @@
         <v>94</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4874,44 +4884,42 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>82</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>83</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="P30" t="s" s="2">
-        <v>261</v>
-      </c>
+      <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
         <v>74</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>262</v>
+        <v>74</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>74</v>
@@ -4950,7 +4958,7 @@
         <v>74</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>75</v>
@@ -4965,15 +4973,15 @@
         <v>94</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>264</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4981,7 +4989,7 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>82</v>
@@ -4990,33 +4998,35 @@
         <v>83</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>83</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="P31" s="2"/>
+      <c r="P31" t="s" s="2">
+        <v>264</v>
+      </c>
       <c r="Q31" t="s" s="2">
         <v>74</v>
       </c>
       <c r="R31" t="s" s="2">
-        <v>74</v>
+        <v>265</v>
       </c>
       <c r="S31" t="s" s="2">
         <v>74</v>
@@ -5055,7 +5065,7 @@
         <v>74</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>75</v>
@@ -5070,23 +5080,23 @@
         <v>94</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>74</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>272</v>
+        <v>74</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F32" t="s" s="2">
         <v>82</v>
@@ -5101,16 +5111,16 @@
         <v>83</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>220</v>
+        <v>269</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5136,11 +5146,13 @@
         <v>74</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="X32" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="Y32" t="s" s="2">
-        <v>276</v>
+        <v>74</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>74</v>
@@ -5158,13 +5170,13 @@
         <v>74</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>74</v>
@@ -5173,26 +5185,26 @@
         <v>94</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>278</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>83</v>
@@ -5204,15 +5216,17 @@
         <v>83</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>277</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>278</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>74</v>
@@ -5241,7 +5255,7 @@
       </c>
       <c r="X33" s="2"/>
       <c r="Y33" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>74</v>
@@ -5259,7 +5273,7 @@
         <v>74</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>75</v>
@@ -5274,19 +5288,19 @@
         <v>94</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>74</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>74</v>
+        <v>283</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5305,13 +5319,13 @@
         <v>83</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5338,11 +5352,11 @@
         <v>74</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="X34" s="2"/>
       <c r="Y34" t="s" s="2">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>74</v>
@@ -5360,7 +5374,7 @@
         <v>74</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>75</v>
@@ -5375,7 +5389,7 @@
         <v>94</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>74</v>
@@ -5383,7 +5397,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5406,13 +5420,13 @@
         <v>83</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5439,13 +5453,11 @@
         <v>74</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X35" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="X35" s="2"/>
       <c r="Y35" t="s" s="2">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>74</v>
@@ -5463,7 +5475,7 @@
         <v>74</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>75</v>
@@ -5478,15 +5490,15 @@
         <v>94</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>294</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5497,7 +5509,7 @@
         <v>75</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>83</v>
@@ -5509,13 +5521,13 @@
         <v>83</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>84</v>
+        <v>293</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5566,13 +5578,13 @@
         <v>74</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>74</v>
@@ -5581,15 +5593,15 @@
         <v>94</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>74</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5615,14 +5627,12 @@
         <v>84</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="L37" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>302</v>
-      </c>
+      <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>74</v>
@@ -5671,7 +5681,7 @@
         <v>74</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>75</v>
@@ -5686,15 +5696,15 @@
         <v>94</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5708,24 +5718,26 @@
         <v>82</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K38" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>74</v>
@@ -5774,7 +5786,7 @@
         <v>74</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>75</v>
@@ -5789,7 +5801,7 @@
         <v>94</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>74</v>
@@ -5797,7 +5809,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5817,16 +5829,16 @@
         <v>74</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="K39" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5877,7 +5889,7 @@
         <v>74</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>75</v>
@@ -5892,15 +5904,15 @@
         <v>94</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5911,29 +5923,27 @@
         <v>75</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I40" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="H40" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I40" t="s" s="2">
-        <v>74</v>
-      </c>
       <c r="J40" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="K40" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>318</v>
-      </c>
+      <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>74</v>
@@ -5982,13 +5992,13 @@
         <v>74</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>74</v>
@@ -5997,15 +6007,15 @@
         <v>94</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6016,10 +6026,10 @@
         <v>75</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>74</v>
@@ -6028,15 +6038,17 @@
         <v>74</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>84</v>
+        <v>318</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>96</v>
+        <v>319</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="M41" s="2"/>
+        <v>320</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>321</v>
+      </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>74</v>
@@ -6085,22 +6097,22 @@
         <v>74</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>98</v>
+        <v>317</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>99</v>
+        <v>322</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>74</v>
@@ -6108,18 +6120,18 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>74</v>
@@ -6131,17 +6143,15 @@
         <v>74</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>74</v>
@@ -6178,31 +6188,31 @@
         <v>74</v>
       </c>
       <c r="AA42" t="s" s="2">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="AB42" t="s" s="2">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="AC42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AD42" t="s" s="2">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>99</v>
@@ -6211,15 +6221,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="B43" t="s" s="2">
-        <v>322</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6229,7 +6237,7 @@
         <v>76</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>74</v>
@@ -6238,15 +6246,17 @@
         <v>74</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>323</v>
+        <v>102</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>324</v>
+        <v>103</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="M43" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>74</v>
@@ -6283,16 +6293,16 @@
         <v>74</v>
       </c>
       <c r="AA43" t="s" s="2">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="AB43" t="s" s="2">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="AC43" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AD43" t="s" s="2">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="AE43" t="s" s="2">
         <v>109</v>
@@ -6310,7 +6320,7 @@
         <v>110</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>74</v>
@@ -6318,10 +6328,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C44" t="s" s="2">
         <v>74</v>
@@ -6343,13 +6353,13 @@
         <v>74</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="K44" t="s" s="2">
         <v>327</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="L44" t="s" s="2">
         <v>328</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6423,9 +6433,11 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="B45" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>329</v>
+      </c>
       <c r="C45" t="s" s="2">
         <v>74</v>
       </c>
@@ -6434,7 +6446,7 @@
         <v>75</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>83</v>
@@ -6443,10 +6455,10 @@
         <v>74</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>158</v>
+        <v>330</v>
       </c>
       <c r="K45" t="s" s="2">
         <v>331</v>
@@ -6479,13 +6491,13 @@
         <v>74</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>214</v>
+        <v>74</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>333</v>
+        <v>74</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>334</v>
+        <v>74</v>
       </c>
       <c r="Z45" t="s" s="2">
         <v>74</v>
@@ -6503,22 +6515,22 @@
         <v>74</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>335</v>
+        <v>109</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>336</v>
+        <v>74</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>337</v>
+        <v>74</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>74</v>
@@ -6526,7 +6538,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6549,20 +6561,16 @@
         <v>83</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>342</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>74</v>
       </c>
@@ -6586,13 +6594,13 @@
         <v>74</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>74</v>
+        <v>217</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>74</v>
+        <v>336</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>74</v>
+        <v>337</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>74</v>
@@ -6610,7 +6618,7 @@
         <v>74</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>75</v>
@@ -6619,21 +6627,21 @@
         <v>82</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>74</v>
+        <v>339</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>94</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="47" hidden="true">
+    <row r="47">
       <c r="A47" t="s" s="2">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6647,28 +6655,28 @@
         <v>82</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>83</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>74</v>
@@ -6693,13 +6701,13 @@
         <v>74</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>214</v>
+        <v>74</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>350</v>
+        <v>74</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>351</v>
+        <v>74</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>74</v>
@@ -6717,7 +6725,7 @@
         <v>74</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>75</v>
@@ -6732,7 +6740,7 @@
         <v>94</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>74</v>
@@ -6740,7 +6748,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6757,24 +6765,26 @@
         <v>74</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>83</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>355</v>
+        <v>158</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="N48" s="2"/>
+        <v>351</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>352</v>
+      </c>
       <c r="O48" t="s" s="2">
         <v>74</v>
       </c>
@@ -6798,13 +6808,13 @@
         <v>74</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>74</v>
+        <v>217</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>74</v>
+        <v>353</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>74</v>
+        <v>354</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>74</v>
@@ -6822,7 +6832,7 @@
         <v>74</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>75</v>
@@ -6837,7 +6847,7 @@
         <v>94</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>99</v>
+        <v>356</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>74</v>
@@ -6845,7 +6855,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6868,15 +6878,17 @@
         <v>83</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>244</v>
+        <v>358</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>361</v>
       </c>
-      <c r="L49" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>74</v>
@@ -6925,7 +6937,7 @@
         <v>74</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>75</v>
@@ -6940,15 +6952,15 @@
         <v>94</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>364</v>
+        <v>99</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6959,29 +6971,27 @@
         <v>75</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I50" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="H50" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>74</v>
-      </c>
       <c r="J50" t="s" s="2">
-        <v>290</v>
+        <v>247</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>368</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>74</v>
@@ -7030,13 +7040,13 @@
         <v>74</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>74</v>
@@ -7045,15 +7055,15 @@
         <v>94</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="51" hidden="true">
+    <row r="51">
       <c r="A51" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7067,7 +7077,7 @@
         <v>76</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>74</v>
@@ -7076,16 +7086,16 @@
         <v>74</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7111,13 +7121,13 @@
         <v>74</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>372</v>
+        <v>74</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>374</v>
+        <v>74</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>74</v>
@@ -7135,7 +7145,7 @@
         <v>74</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>75</v>
@@ -7150,7 +7160,7 @@
         <v>94</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>74</v>
@@ -7158,7 +7168,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7181,15 +7191,17 @@
         <v>74</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>377</v>
+        <v>223</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="M52" s="2"/>
+        <v>375</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>376</v>
+      </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>74</v>
@@ -7214,13 +7226,13 @@
         <v>74</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>74</v>
+        <v>375</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>74</v>
+        <v>377</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>74</v>
@@ -7238,7 +7250,7 @@
         <v>74</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>75</v>
@@ -7253,7 +7265,7 @@
         <v>94</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>74</v>
+        <v>378</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>74</v>
@@ -7261,7 +7273,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7272,7 +7284,7 @@
         <v>75</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>74</v>
@@ -7284,13 +7296,13 @@
         <v>74</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>84</v>
+        <v>380</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>96</v>
+        <v>381</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>97</v>
+        <v>382</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7341,22 +7353,22 @@
         <v>74</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>98</v>
+        <v>379</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="AK53" t="s" s="2">
         <v>74</v>
@@ -7364,18 +7376,18 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>74</v>
@@ -7387,17 +7399,15 @@
         <v>74</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
         <v>74</v>
@@ -7446,19 +7456,19 @@
         <v>74</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>99</v>
@@ -7469,11 +7479,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>383</v>
+        <v>101</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7486,26 +7496,24 @@
         <v>74</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J55" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>384</v>
+        <v>103</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>385</v>
+        <v>104</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="N55" t="s" s="2">
-        <v>199</v>
-      </c>
+      <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
         <v>74</v>
       </c>
@@ -7553,7 +7561,7 @@
         <v>74</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>386</v>
+        <v>109</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>75</v>
@@ -7568,7 +7576,7 @@
         <v>110</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>74</v>
@@ -7576,39 +7584,43 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>74</v>
+        <v>386</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>74</v>
       </c>
       <c r="H56" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>220</v>
+        <v>102</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L56" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
+      <c r="M56" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>202</v>
+      </c>
       <c r="O56" t="s" s="2">
         <v>74</v>
       </c>
@@ -7632,10 +7644,10 @@
         <v>74</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>390</v>
+        <v>74</v>
       </c>
       <c r="Y56" t="s" s="2">
         <v>74</v>
@@ -7656,22 +7668,22 @@
         <v>74</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>375</v>
+        <v>181</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>74</v>
@@ -7679,7 +7691,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7702,17 +7714,15 @@
         <v>74</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>305</v>
+        <v>223</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="L57" t="s" s="2">
-        <v>393</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>394</v>
-      </c>
+      <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>74</v>
@@ -7737,10 +7747,10 @@
         <v>74</v>
       </c>
       <c r="W57" t="s" s="2">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>74</v>
+        <v>393</v>
       </c>
       <c r="Y57" t="s" s="2">
         <v>74</v>
@@ -7761,7 +7771,7 @@
         <v>74</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>75</v>
@@ -7776,7 +7786,7 @@
         <v>94</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>74</v>
@@ -7784,7 +7794,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7795,7 +7805,7 @@
         <v>75</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>74</v>
@@ -7807,16 +7817,16 @@
         <v>74</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>220</v>
+        <v>308</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>397</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -7842,13 +7852,13 @@
         <v>74</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>400</v>
+        <v>74</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>401</v>
+        <v>74</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>74</v>
@@ -7866,13 +7876,13 @@
         <v>74</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>74</v>
@@ -7881,7 +7891,7 @@
         <v>94</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>74</v>
@@ -7889,7 +7899,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7912,16 +7922,16 @@
         <v>74</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -7950,10 +7960,10 @@
         <v>148</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>74</v>
+        <v>404</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>74</v>
@@ -7971,7 +7981,7 @@
         <v>74</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>75</v>
@@ -7986,7 +7996,7 @@
         <v>94</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>74</v>
@@ -7994,7 +8004,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8017,16 +8027,16 @@
         <v>74</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="M60" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -8052,13 +8062,13 @@
         <v>74</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>163</v>
+        <v>410</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>74</v>
@@ -8076,7 +8086,7 @@
         <v>74</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>75</v>
@@ -8091,7 +8101,7 @@
         <v>94</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>74</v>
+        <v>405</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>74</v>
@@ -8099,7 +8109,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8122,15 +8132,17 @@
         <v>74</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>413</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>414</v>
       </c>
-      <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>74</v>
@@ -8155,13 +8167,13 @@
         <v>74</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>415</v>
+        <v>163</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>416</v>
+        <v>164</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>74</v>
@@ -8179,7 +8191,7 @@
         <v>74</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>75</v>
@@ -8194,15 +8206,15 @@
         <v>94</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>402</v>
+        <v>74</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8213,10 +8225,10 @@
         <v>75</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>74</v>
@@ -8225,13 +8237,13 @@
         <v>74</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8258,13 +8270,13 @@
         <v>74</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>74</v>
+        <v>418</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>74</v>
+        <v>419</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>74</v>
@@ -8282,13 +8294,13 @@
         <v>74</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>74</v>
@@ -8297,7 +8309,7 @@
         <v>94</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="AK62" t="s" s="2">
         <v>74</v>
@@ -8316,7 +8328,7 @@
         <v>75</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>83</v>
@@ -8328,7 +8340,7 @@
         <v>74</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>377</v>
+        <v>260</v>
       </c>
       <c r="K63" t="s" s="2">
         <v>421</v>
@@ -8336,9 +8348,7 @@
       <c r="L63" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="M63" t="s" s="2">
-        <v>423</v>
-      </c>
+      <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>74</v>
@@ -8393,7 +8403,7 @@
         <v>75</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>74</v>
@@ -8402,15 +8412,15 @@
         <v>94</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="AK63" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="64" hidden="true">
+    <row r="64">
       <c r="A64" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8421,10 +8431,10 @@
         <v>75</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>74</v>
@@ -8433,15 +8443,17 @@
         <v>74</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>84</v>
+        <v>380</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>96</v>
+        <v>424</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="M64" s="2"/>
+        <v>425</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>426</v>
+      </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>74</v>
@@ -8490,22 +8502,22 @@
         <v>74</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>98</v>
+        <v>423</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>99</v>
+        <v>427</v>
       </c>
       <c r="AK64" t="s" s="2">
         <v>74</v>
@@ -8513,18 +8525,18 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>74</v>
@@ -8536,17 +8548,15 @@
         <v>74</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>74</v>
@@ -8595,19 +8605,19 @@
         <v>74</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>99</v>
@@ -8618,11 +8628,11 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>383</v>
+        <v>101</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
@@ -8635,26 +8645,24 @@
         <v>74</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J66" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>384</v>
+        <v>103</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>385</v>
+        <v>104</v>
       </c>
       <c r="M66" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="N66" t="s" s="2">
-        <v>199</v>
-      </c>
+      <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>74</v>
       </c>
@@ -8702,7 +8710,7 @@
         <v>74</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>386</v>
+        <v>109</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>75</v>
@@ -8717,19 +8725,19 @@
         <v>110</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>74</v>
+        <v>386</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
@@ -8739,25 +8747,29 @@
         <v>76</v>
       </c>
       <c r="G67" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H67" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="H67" t="s" s="2">
-        <v>74</v>
-      </c>
       <c r="I67" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>429</v>
+        <v>387</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
+        <v>388</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N67" t="s" s="2">
+        <v>202</v>
+      </c>
       <c r="O67" t="s" s="2">
         <v>74</v>
       </c>
@@ -8781,13 +8793,13 @@
         <v>74</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>214</v>
+        <v>74</v>
       </c>
       <c r="X67" t="s" s="2">
-        <v>431</v>
+        <v>74</v>
       </c>
       <c r="Y67" t="s" s="2">
-        <v>432</v>
+        <v>74</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>74</v>
@@ -8805,7 +8817,7 @@
         <v>74</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>428</v>
+        <v>389</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>75</v>
@@ -8817,10 +8829,10 @@
         <v>74</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>424</v>
+        <v>181</v>
       </c>
       <c r="AK67" t="s" s="2">
         <v>74</v>
@@ -8828,7 +8840,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8839,7 +8851,7 @@
         <v>75</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>83</v>
@@ -8851,13 +8863,13 @@
         <v>74</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>257</v>
+        <v>158</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8884,13 +8896,13 @@
         <v>74</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>74</v>
+        <v>217</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>74</v>
+        <v>434</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>74</v>
+        <v>435</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>74</v>
@@ -8908,13 +8920,13 @@
         <v>74</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>74</v>
@@ -8923,7 +8935,7 @@
         <v>94</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>74</v>
@@ -8954,17 +8966,15 @@
         <v>74</v>
       </c>
       <c r="J69" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="K69" t="s" s="2">
         <v>437</v>
       </c>
-      <c r="K69" t="s" s="2">
+      <c r="L69" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="L69" t="s" s="2">
-        <v>439</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>440</v>
-      </c>
+      <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>74</v>
@@ -9028,7 +9038,7 @@
         <v>94</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>74</v>
@@ -9036,7 +9046,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9059,16 +9069,16 @@
         <v>74</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -9118,7 +9128,7 @@
         <v>74</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>75</v>
@@ -9133,7 +9143,7 @@
         <v>94</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>74</v>
@@ -9152,7 +9162,7 @@
         <v>75</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>83</v>
@@ -9164,7 +9174,7 @@
         <v>74</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>377</v>
+        <v>440</v>
       </c>
       <c r="K71" t="s" s="2">
         <v>445</v>
@@ -9172,7 +9182,9 @@
       <c r="L71" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="M71" s="2"/>
+      <c r="M71" t="s" s="2">
+        <v>443</v>
+      </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
         <v>74</v>
@@ -9227,7 +9239,7 @@
         <v>75</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH71" t="s" s="2">
         <v>74</v>
@@ -9236,13 +9248,13 @@
         <v>94</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="72" hidden="true">
+    <row r="72">
       <c r="A72" t="s" s="2">
         <v>447</v>
       </c>
@@ -9255,10 +9267,10 @@
         <v>75</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H72" t="s" s="2">
         <v>74</v>
@@ -9267,13 +9279,13 @@
         <v>74</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>84</v>
+        <v>380</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>96</v>
+        <v>448</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>97</v>
+        <v>449</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -9324,22 +9336,22 @@
         <v>74</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>98</v>
+        <v>447</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>99</v>
+        <v>427</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>74</v>
@@ -9347,18 +9359,18 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>74</v>
@@ -9370,17 +9382,15 @@
         <v>74</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
         <v>74</v>
@@ -9429,19 +9439,19 @@
         <v>74</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="AJ73" t="s" s="2">
         <v>99</v>
@@ -9452,11 +9462,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>383</v>
+        <v>101</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9469,26 +9479,24 @@
         <v>74</v>
       </c>
       <c r="H74" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J74" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>384</v>
+        <v>103</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>385</v>
+        <v>104</v>
       </c>
       <c r="M74" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="N74" t="s" s="2">
-        <v>199</v>
-      </c>
+      <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
         <v>74</v>
       </c>
@@ -9536,7 +9544,7 @@
         <v>74</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>386</v>
+        <v>109</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>75</v>
@@ -9551,47 +9559,51 @@
         <v>110</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>74</v>
+        <v>386</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G75" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H75" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="H75" t="s" s="2">
-        <v>74</v>
-      </c>
       <c r="I75" t="s" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>451</v>
+        <v>387</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>452</v>
-      </c>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
+        <v>388</v>
+      </c>
+      <c r="M75" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N75" t="s" s="2">
+        <v>202</v>
+      </c>
       <c r="O75" t="s" s="2">
         <v>74</v>
       </c>
@@ -9639,22 +9651,22 @@
         <v>74</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>450</v>
+        <v>389</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>99</v>
+        <v>181</v>
       </c>
       <c r="AK75" t="s" s="2">
         <v>74</v>
@@ -9670,7 +9682,7 @@
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F76" t="s" s="2">
         <v>82</v>
@@ -9685,7 +9697,7 @@
         <v>74</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>244</v>
+        <v>84</v>
       </c>
       <c r="K76" t="s" s="2">
         <v>454</v>
@@ -9745,7 +9757,7 @@
         <v>453</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>82</v>
@@ -9757,7 +9769,7 @@
         <v>94</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>424</v>
+        <v>99</v>
       </c>
       <c r="AK76" t="s" s="2">
         <v>74</v>
@@ -9788,7 +9800,7 @@
         <v>74</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>84</v>
+        <v>247</v>
       </c>
       <c r="K77" t="s" s="2">
         <v>457</v>
@@ -9860,7 +9872,7 @@
         <v>94</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>74</v>
@@ -9879,7 +9891,7 @@
         <v>75</v>
       </c>
       <c r="F78" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G78" t="s" s="2">
         <v>83</v>
@@ -9891,13 +9903,13 @@
         <v>74</v>
       </c>
       <c r="J78" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="K78" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="K78" t="s" s="2">
+      <c r="L78" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>462</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -9954,7 +9966,7 @@
         <v>75</v>
       </c>
       <c r="AG78" t="s" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AH78" t="s" s="2">
         <v>74</v>
@@ -9963,14 +9975,117 @@
         <v>94</v>
       </c>
       <c r="AJ78" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="AK78" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F79" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G79" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J79" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="K79" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="L79" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P79" s="2"/>
+      <c r="Q79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE79" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="AF79" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG79" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH79" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI79" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AJ79" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AK78" t="s" s="2">
+      <c r="AK79" t="s" s="2">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK78">
+  <autoFilter ref="A1:AK79">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9980,7 +10095,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI77">
+  <conditionalFormatting sqref="A2:AI78">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>